<commit_message>
Reading excel File Completed
</commit_message>
<xml_diff>
--- a/excel/NameData.xlsx
+++ b/excel/NameData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="name" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t xml:space="preserve">Shraddha</t>
   </si>
@@ -121,36 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">Brilio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0    (x,y)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,3</t>
   </si>
 </sst>
 </file>
@@ -253,11 +223,11 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -396,50 +366,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.93"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>36</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>40</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>41</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>42</v>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -464,7 +487,7 @@
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Data Driven Automation Framework
</commit_message>
<xml_diff>
--- a/excel/NameData.xlsx
+++ b/excel/NameData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="name" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t xml:space="preserve">Shraddha</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t xml:space="preserve">Brilio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.google.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twitter. It’s what’s happening / Twitter</t>
   </si>
 </sst>
 </file>
@@ -130,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -151,6 +166,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,12 +217,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,10 +250,10 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -368,11 +394,11 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.93"/>
   </cols>
@@ -481,14 +507,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.google.com/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>